<commit_message>
updated fm24 to use new calcrules
</commit_message>
<xml_diff>
--- a/ftest/data/fm26/target_sidx1.xlsx
+++ b/ftest/data/fm26/target_sidx1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\data\fm26\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{03E6D44F-872F-48C2-A076-FCA535A71D34}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{91319D44-F232-4B33-912E-1FAE3E3954D2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{2D752E1E-D3A9-410B-92F1-07338E7E53EA}"/>
   </bookViews>
@@ -439,7 +439,7 @@
   <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,7 +555,7 @@
         <v>0</v>
       </c>
       <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
+      <c r="Q4" s="1"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
@@ -592,6 +592,7 @@
       <c r="O5">
         <v>0</v>
       </c>
+      <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C6">
@@ -622,6 +623,7 @@
       <c r="O6">
         <v>0</v>
       </c>
+      <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C7">
@@ -652,6 +654,7 @@
       <c r="O7">
         <v>0</v>
       </c>
+      <c r="Q7" s="1"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C8">
@@ -682,6 +685,7 @@
       <c r="O8">
         <v>55777064</v>
       </c>
+      <c r="Q8" s="1"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C9">
@@ -712,6 +716,7 @@
       <c r="O9">
         <v>0</v>
       </c>
+      <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C10">
@@ -742,6 +747,7 @@
       <c r="O10">
         <v>398635.53</v>
       </c>
+      <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C11">
@@ -772,6 +778,7 @@
       <c r="O11">
         <v>5100906</v>
       </c>
+      <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C12">
@@ -802,6 +809,7 @@
       <c r="O12">
         <v>35437872</v>
       </c>
+      <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C13">
@@ -832,6 +840,7 @@
       <c r="O13">
         <v>0</v>
       </c>
+      <c r="Q13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>